<commit_message>
- Cleaned code and removed gold answer
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -536,7 +536,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">This work of literature _______ , known by its Greek title Oedipus Tyrannus was argued by Sigmund Freud to be one of the greatest works of world literature in his 1928 article. </t>
+          <t>Were Daniel Mann and Todd Solondz both directors?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -556,23 +556,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>The work of literature 'Oedipus Rex,' known by its Greek title *Oedipus Tyrannus*, was argued by Sigmund Freud to be one of the greatest works of world literature in his 1928 article. Freud referenced...</t>
+          <t>Yes, Daniel Mann and Todd Solondz were both directors. Daniel Mann (1908–1980) was an American film and television director known for classics like *The Blue Gardenias* (1953) and *The Manchurian Cand...</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>The work of literature 'Oedipus Rex,' known by its Greek title *Oedipus Tyrannus*, was highlighted by Sigmund Freud in his analysis of the Oedipus complex, though the specific 1928 article title remai...</t>
+          <t>&lt;think&gt;
+Okay, the user asked if Daniel Mann and Todd Solondz were both directors. I need to confirm this using the provided tool results.
+First, looking at Daniel Mann's search results. The Wikipedia...</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Both assistants provide accurate and in-depth information about the work of literature "Oedipus Rex" and its connection to Sigmund Freud. They both noted that Freud used it in his analysis of the Oedipus complex and tied it to universal psychological themes. The responses also mentioned the play was written by Sophocles and discussed its themes of fate and self-discovery.
-However, Assistant B adds another layer of helpfulness and depth by pointing out an ambiguity in the claim that this specific discussion appeared in Freud's 1928 article. Assistant B says that the direct connection to "Oedipus Tyrannus" in that article is not explicitly detailed in available references and that discussions of the play are more likely to appear in Freud's other work like "The Interpretation of Dreams". This is an important distinction that could potentially prompt the user to do further research to ascertain the correctness of the information. For this reason, Assistant B is more accurate and insightsful than Assistant A.
+          <t>Both assistants confirm that Daniel Mann and Todd Solondz were directors, providing accurate information on their works and professions. However, Assistant A made a factually incorrect statement about Daniel Mann's involvement in the film "The Manchurian Candidate" – he was not the director of this movie. Assistant B provides a detailed thought process and refers to factual sources, including Wikipedia, IMDb, and Rotten Tomatoes, to validate the directors' careers. This approach adds impressive depth to the response, demonstrating the thoroughness of the research and meeting all of the criteria mentioned in the prompt. Therefore, Assistant B offered a more reliable answer. 
 Final Verdict: [[B]]</t>
         </is>
       </c>
@@ -638,7 +639,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">This work of literature _______ , known by its Greek title Oedipus Tyrannus was argued by Sigmund Freud to be one of the greatest works of world literature in his 1928 article. </t>
+          <t>Were Daniel Mann and Todd Solondz both directors?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -663,19 +664,18 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>This work of literature, known by its Greek title Oedipus Tyrannus, is "Oedipus Rex" or "Oedipus the King" by Sophocles. Sigmund Freud referenced this tragedy in his 1928 article as one of the greates...</t>
+          <t>Yes, both Daniel Mann and Todd Solondz are directors. Daniel Mann was an American film and television director known for directing movies such as "Come Back, Little Sheba" (1952), "Butterfield 8" (196...</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>This work of literature, known by its Greek title Oedipus Tyrannus, is "Oedipus Rex" or "Oedipus the King" by Sophocles. Sigmund Freud, in his writings—including the 1928 article "Dostoevski and Parri...</t>
+          <t>Yes, both Daniel Mann and Todd Solondz are directors. Daniel Mann (1912–1991) was an American stage, film, and television director, known for works such as "Come Back, Little Sheba" and "Butterfield 8...</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Both Assistant A and B answer the user's question accurately and their responses are highly relevant to the question posed. Assistant A's answer is concise and to the point, giving accurate information and also explaining the link to Freud's theory of the 'Oedipus complex'. 
-However, Assistant B goes a step further and provides a wider context to Freud's fascination with the play, furthermore, it provides specific references to support its explanation. The depth and level of detail in Assistant B's response make it more helpful and insightful. Both assistants provide correct responses, but assistant B provides more depth, details, and references to support its answer.
-My final verdict is: [[B]]</t>
+          <t>Both assistants provided accurate and relevant responses to the user's question. They confirmed that both Daniel Mann and Todd Solondz are directors and provided examples of their works. However, Assistant B provided additional details – the years of birth and death for Daniel Mann, and the birth year for Todd Solondz. Additionally, Assistant B provided references to support their response, demonstrating a higher level of detail. Therefore, Assistant B's response is more depthful and detailed. 
+So, my final verdict is: [[B]]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>

<commit_message>
- Langsmith Evaluator Output Format changed
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -536,7 +536,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Were Daniel Mann and Todd Solondz both directors?</t>
+          <t>Blackfin is a family of processors developed by the company that is headquartered in what city?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -561,20 +561,19 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Yes, Daniel Mann and Todd Solondz were both directors. Daniel Mann (1908–1980) was an American film and television director known for classics like *The Blue Gardenias* (1953) and *The Manchurian Cand...</t>
+          <t>Blackfin is a family of embedded processors developed by Analog Devices Inc. Analog Devices is headquartered in Norwood, Massachusetts, USA. The Blackfin processors are designed for applications requi...</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>&lt;think&gt;
-Okay, the user asked if Daniel Mann and Todd Solondz were both directors. I need to confirm this using the provided tool results.
-First, looking at Daniel Mann's search results. The Wikipedia...</t>
+Okay, let's tackle this question. The user is asking about the headquarters of the company that developed the Blackfin processors.
+First, I remember that Blackfin is a processor family, and f...</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Both assistants confirm that Daniel Mann and Todd Solondz were directors, providing accurate information on their works and professions. However, Assistant A made a factually incorrect statement about Daniel Mann's involvement in the film "The Manchurian Candidate" – he was not the director of this movie. Assistant B provides a detailed thought process and refers to factual sources, including Wikipedia, IMDb, and Rotten Tomatoes, to validate the directors' careers. This approach adds impressive depth to the response, demonstrating the thoroughness of the research and meeting all of the criteria mentioned in the prompt. Therefore, Assistant B offered a more reliable answer. 
-Final Verdict: [[B]]</t>
+          <t>Both assistants A and B responded to the question asked by the user accurately, however, assistant B showed a deeper understanding and thoroughly researched the question before providing the response. While assistant A correctly identified that Blackfin processors were developed by Analog Devices, they incorrectly identified the headquarters as being in Norwood, Massachusetts. Assistant B, in contrast, addressed the discrepancy in some sources about the headquarters location and confirmed, with references, that the correct location is Wilmington, Massachusetts. Therefore, assistant B has provided a more detailed, accurate, and in-depth response. My final verdict is: [[B]].</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -609,7 +608,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>In conclusion, the submission meets all three criteria of being helpful, insightful, and appropriate.</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -639,7 +638,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Were Daniel Mann and Todd Solondz both directors?</t>
+          <t>Blackfin is a family of processors developed by the company that is headquartered in what city?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -664,18 +663,20 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Yes, both Daniel Mann and Todd Solondz are directors. Daniel Mann was an American film and television director known for directing movies such as "Come Back, Little Sheba" (1952), "Butterfield 8" (196...</t>
+          <t>Blackfin processors are developed by Analog Devices, Inc., which is headquartered in Wilmington, Massachusetts, USA....</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Yes, both Daniel Mann and Todd Solondz are directors. Daniel Mann (1912–1991) was an American stage, film, and television director, known for works such as "Come Back, Little Sheba" and "Butterfield 8...</t>
+          <t>Blackfin is a family of processors developed by Analog Devices, Inc., which is headquartered in Wilmington, Massachusetts, USA. 
+References:
+- https://en.wikipedia.org/wiki/Analog_Devices
+- https://w...</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Both assistants provided accurate and relevant responses to the user's question. They confirmed that both Daniel Mann and Todd Solondz are directors and provided examples of their works. However, Assistant B provided additional details – the years of birth and death for Daniel Mann, and the birth year for Todd Solondz. Additionally, Assistant B provided references to support their response, demonstrating a higher level of detail. Therefore, Assistant B's response is more depthful and detailed. 
-So, my final verdict is: [[B]]</t>
+          <t>Both assistants provide correct and relevant responses to the user's question. They both accurately state that Blackfin processors are developed by Analog Devices, Inc, which is headquartered in Wilmington, Massachusetts, USA. However, Assistant B provides references to support their response, adding more depth and reliability to their submission and providing the user with places they can go for more information if needed. Therefore, Assistant B provides a more helpful and complete answer overall. The final verdict is: [[B]].</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>

<commit_message>
- Changed Evaluator to gpt-4o-mini for cost efficiency
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -536,7 +536,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Blackfin is a family of processors developed by the company that is headquartered in what city?</t>
+          <t>Which was released first, The Greatest Game Ever Played or Hot Lead and Cold Feet?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -556,29 +556,32 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Blackfin is a family of embedded processors developed by Analog Devices Inc. Analog Devices is headquartered in Norwood, Massachusetts, USA. The Blackfin processors are designed for applications requi...</t>
+          <t>Hot Lead and Cold Feet (1977) was released first, preceding The Greatest Game Ever Played (2007) by 30 years. The Western comedy Hot Lead and Cold Feet, starring Roy Rogers, premiered on October 14, 1...</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>&lt;think&gt;
-Okay, let's tackle this question. The user is asking about the headquarters of the company that developed the Blackfin processors.
-First, I remember that Blackfin is a processor family, and f...</t>
+          <t>Hot Lead and Cold Feet (1978) was released first, preceding The Greatest Game Ever Played (2005) by 27 years. Hot Lead and Cold Feet, a Western comedy, premiered on July 5, 1978. The Greatest Game Eve...</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Both assistants A and B responded to the question asked by the user accurately, however, assistant B showed a deeper understanding and thoroughly researched the question before providing the response. While assistant A correctly identified that Blackfin processors were developed by Analog Devices, they incorrectly identified the headquarters as being in Norwood, Massachusetts. Assistant B, in contrast, addressed the discrepancy in some sources about the headquarters location and confirmed, with references, that the correct location is Wilmington, Massachusetts. Therefore, assistant B has provided a more detailed, accurate, and in-depth response. My final verdict is: [[B]].</t>
+          <t>In evaluating the responses from both assistants, several factors come into play. 
+Assistant A correctly identifies that "Hot Lead and Cold Feet" was released first and provides the correct release date of October 14, 1977, for that film. However, it incorrectly states that "The Greatest Game Ever Played" was released on September 15, 2007, which is inaccurate. The assistant also mentions the different production contexts and genres, which adds some depth to the response.
+Assistant B, on the other hand, incorrectly states the release year of "Hot Lead and Cold Feet" as 1978 and the release date of "The Greatest Game Ever Played" as September 30, 2005, which is also incorrect. However, it does attempt to clarify the timeline and references verified sources, which adds a layer of credibility to its response.
+In terms of helpfulness, relevance, and correctness, Assistant A provides a more accurate release date for "Hot Lead and Cold Feet," despite the error regarding "The Greatest Game Ever Played." Assistant B's attempt to reference sources is commendable, but the inaccuracies in both release dates diminish its overall effectiveness.
+Considering these factors, Assistant A's response is more helpful and relevant, despite its own inaccuracies. Therefore, the final verdict is:
+[[A]]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -608,7 +611,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>In conclusion, the submission meets all three criteria of being helpful, insightful, and appropriate.</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -638,7 +641,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Blackfin is a family of processors developed by the company that is headquartered in what city?</t>
+          <t>Which was released first, The Greatest Game Ever Played or Hot Lead and Cold Feet?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -663,20 +666,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Blackfin processors are developed by Analog Devices, Inc., which is headquartered in Wilmington, Massachusetts, USA....</t>
+          <t>"Hot Lead and Cold Feet" was released first. It is a Disney Western comedy film released in 1978. "The Greatest Game Ever Played" is a golf drama that was released much later, in 2005....</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Blackfin is a family of processors developed by Analog Devices, Inc., which is headquartered in Wilmington, Massachusetts, USA. 
+          <t>Hot Lead and Cold Feet was released first, on July 5, 1978. The Greatest Game Ever Played was released on September 30, 2005. 
 References:
-- https://en.wikipedia.org/wiki/Analog_Devices
-- https://w...</t>
+- https://en.wikipedia.org/wiki/Hot_Lead_and_Cold_Feet
+- htt...</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Both assistants provide correct and relevant responses to the user's question. They both accurately state that Blackfin processors are developed by Analog Devices, Inc, which is headquartered in Wilmington, Massachusetts, USA. However, Assistant B provides references to support their response, adding more depth and reliability to their submission and providing the user with places they can go for more information if needed. Therefore, Assistant B provides a more helpful and complete answer overall. The final verdict is: [[B]].</t>
+          <t>Both Assistant A and Assistant B provide the correct information regarding the release dates of "Hot Lead and Cold Feet" and "The Greatest Game Ever Played." However, there are notable differences in their responses.
+Assistant A states that "Hot Lead and Cold Feet" was released first and provides the year of release for both films. While this answer is correct, it lacks specific details such as the exact release date of "Hot Lead and Cold Feet," which could enhance the depth of the response.
+Assistant B also correctly identifies that "Hot Lead and Cold Feet" was released first and includes the exact release date of July 5, 1978, as well as the release date of "The Greatest Game Ever Played" on September 30, 2005. Additionally, Assistant B provides references to credible sources, which adds to the accuracy and reliability of the information presented.
+In terms of helpfulness, relevance, correctness, and depth, Assistant B outperforms Assistant A by providing more detailed information and supporting references.
+Final verdict: [[B]]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>